<commit_message>
updating files to acommodate adding drugs 77,81,84
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/figure_making/drug_phylogeny_summary/expanded_drug_info_for_mouse_protocol.xlsx
+++ b/jupyter_notebooks/figure_making/drug_phylogeny_summary/expanded_drug_info_for_mouse_protocol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgvg9\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgvg9\Downloads\ginsparg_thymelab_thesis\jupyter_notebooks\figure_making\drug_phylogeny_summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E282E2-D46E-437C-A51E-3FC8C07032A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5830AF83-AD66-488D-9412-63A68DED3B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="1560" windowWidth="21600" windowHeight="13035" xr2:uid="{3D26C0FB-13FB-4DAD-A6D5-12287546F906}"/>
+    <workbookView xWindow="1230" yWindow="1500" windowWidth="21600" windowHeight="13035" xr2:uid="{3D26C0FB-13FB-4DAD-A6D5-12287546F906}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>enamine_name</t>
   </si>
@@ -177,13 +177,31 @@
   </si>
   <si>
     <t>C19H17N3O2S2</t>
+  </si>
+  <si>
+    <t>Z1438098873</t>
+  </si>
+  <si>
+    <t>CC1(C)CN(C1C=2C=CC=CC2)S(=O)(=O)C3=CC=CC4=NON=C34</t>
+  </si>
+  <si>
+    <t>Z3474884733</t>
+  </si>
+  <si>
+    <t>CC1=CON=C1CS(=O)(=O)N2CCCC2(C)C=3C=CC=CC3</t>
+  </si>
+  <si>
+    <t>Z1271390920</t>
+  </si>
+  <si>
+    <t>COC=1C=CC=CC1CC(C)N(C)S(=O)(=O)C=2C=NN(C2)C(C)C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +213,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -218,9 +242,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7610148-5977-4E68-BA3F-C3F99CA58F7E}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,6 +802,48 @@
         <v>46</v>
       </c>
     </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12">
+        <v>77</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>81</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>